<commit_message>
final edits to first draft of prioritization docs
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230814.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230814.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D5C2F3-CC53-490D-BFDD-ACB4AF673DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436C5601-D02E-49A8-A3DD-CC3BB51EA3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80280" yWindow="-6315" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="validation" sheetId="7" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SR_IPTDS_Sites!$A$1:$AI$101</definedName>
     <definedName name="figure_1_outcomes">validation!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -4372,10 +4373,10 @@
   <dimension ref="A1:AI101"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:AI1"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added comment re: SW1 and SW2
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230814.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230814.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436C5601-D02E-49A8-A3DD-CC3BB51EA3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A67ADF6-6E90-48DA-BF58-7E3696C0FF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80280" yWindow="-6315" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80280" yWindow="-6315" windowWidth="16440" windowHeight="28590" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -3625,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A42020D-9532-4D3F-8F80-EE8C6D0895CA}">
   <dimension ref="B1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4370,13 +4370,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4525,7 +4526,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
@@ -5013,7 +5014,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>231</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>45</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
@@ -5689,7 +5690,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>47</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>48</v>
       </c>
@@ -5891,7 +5892,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>50</v>
       </c>
@@ -5991,7 +5992,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>49</v>
       </c>
@@ -6187,7 +6188,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>55</v>
       </c>
@@ -6287,7 +6288,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>56</v>
       </c>
@@ -6559,7 +6560,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>59</v>
       </c>
@@ -6659,7 +6660,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>60</v>
       </c>
@@ -6759,7 +6760,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>52</v>
       </c>
@@ -6857,7 +6858,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
@@ -6957,7 +6958,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>54</v>
       </c>
@@ -7457,7 +7458,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>63</v>
       </c>
@@ -7557,7 +7558,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>91</v>
       </c>
@@ -7657,7 +7658,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>92</v>
       </c>
@@ -7757,7 +7758,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -7857,7 +7858,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>94</v>
       </c>
@@ -7957,7 +7958,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>64</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
         <v>65</v>
       </c>
@@ -8155,7 +8156,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>70</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>66</v>
       </c>
@@ -8563,7 +8564,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>68</v>
       </c>
@@ -8663,7 +8664,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>67</v>
       </c>
@@ -8765,7 +8766,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>69</v>
       </c>
@@ -8965,7 +8966,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>86</v>
       </c>
@@ -9063,7 +9064,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>90</v>
       </c>
@@ -9161,7 +9162,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>88</v>
       </c>
@@ -9259,7 +9260,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>89</v>
       </c>
@@ -9357,7 +9358,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
         <v>87</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>84</v>
       </c>
@@ -9555,7 +9556,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>367</v>
       </c>
@@ -9639,7 +9640,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>85</v>
       </c>
@@ -9739,7 +9740,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>121</v>
       </c>
@@ -9841,7 +9842,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>120</v>
       </c>
@@ -9941,7 +9942,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>100</v>
       </c>
@@ -10039,7 +10040,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>101</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>104</v>
       </c>
@@ -10239,7 +10240,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>387</v>
       </c>
@@ -10325,7 +10326,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>390</v>
       </c>
@@ -10411,7 +10412,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
         <v>394</v>
       </c>
@@ -10497,7 +10498,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
         <v>106</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
         <v>400</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
         <v>105</v>
       </c>
@@ -10781,7 +10782,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>107</v>
       </c>
@@ -10879,7 +10880,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
         <v>108</v>
       </c>
@@ -10979,7 +10980,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
         <v>109</v>
       </c>
@@ -11077,7 +11078,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
         <v>416</v>
       </c>
@@ -11163,7 +11164,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
         <v>103</v>
       </c>
@@ -11263,7 +11264,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
         <v>102</v>
       </c>
@@ -11363,7 +11364,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
         <v>110</v>
       </c>
@@ -11463,7 +11464,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
         <v>111</v>
       </c>
@@ -11561,7 +11562,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
         <v>112</v>
       </c>
@@ -11661,7 +11662,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>113</v>
       </c>
@@ -11759,7 +11760,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>437</v>
       </c>
@@ -11843,7 +11844,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>114</v>
       </c>
@@ -11943,7 +11944,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>115</v>
       </c>
@@ -12041,7 +12042,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
         <v>116</v>
       </c>
@@ -12139,7 +12140,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>117</v>
       </c>
@@ -12239,7 +12240,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>118</v>
       </c>
@@ -12339,7 +12340,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>454</v>
       </c>
@@ -12423,7 +12424,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>122</v>
       </c>
@@ -12521,7 +12522,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>123</v>
       </c>
@@ -12621,7 +12622,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>124</v>
       </c>
@@ -12723,7 +12724,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
         <v>467</v>
       </c>
@@ -12807,7 +12808,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
         <v>125</v>
       </c>
@@ -12905,7 +12906,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
         <v>126</v>
       </c>
@@ -13003,7 +13004,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
         <v>127</v>
       </c>
@@ -13103,7 +13104,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>73</v>
       </c>
@@ -13203,7 +13204,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="17" t="s">
         <v>82</v>
       </c>
@@ -13303,7 +13304,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>74</v>
       </c>
@@ -13403,7 +13404,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
         <v>75</v>
       </c>
@@ -13689,7 +13690,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="17" t="s">
         <v>77</v>
       </c>
@@ -13789,7 +13790,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="17" t="s">
         <v>78</v>
       </c>
@@ -14089,7 +14090,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="17" t="s">
         <v>81</v>
       </c>
@@ -14191,7 +14192,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="17" t="s">
         <v>83</v>
       </c>
@@ -14294,6 +14295,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI101" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="20">
+      <filters>
+        <filter val="NPT"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -14304,7 +14317,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D18" sqref="D18"/>

</xml_diff>

<commit_message>
added a version of the IPTDS leaflet with HUC10s polygons added
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230814.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230814.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A67ADF6-6E90-48DA-BF58-7E3696C0FF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04DB49B-CC16-431F-90FA-51B671E2F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80280" yWindow="-6315" windowWidth="16440" windowHeight="28590" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -4370,14 +4370,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A99" sqref="A8:XFD99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4526,7 +4525,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>95</v>
       </c>
@@ -4624,7 +4623,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
@@ -4722,7 +4721,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>97</v>
       </c>
@@ -4820,7 +4819,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>98</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>99</v>
       </c>
@@ -5014,7 +5013,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>231</v>
       </c>
@@ -5492,7 +5491,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>45</v>
       </c>
@@ -5592,7 +5591,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
@@ -5690,7 +5689,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>47</v>
       </c>
@@ -5792,7 +5791,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>48</v>
       </c>
@@ -5892,7 +5891,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>50</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>49</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>55</v>
       </c>
@@ -6288,7 +6287,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>56</v>
       </c>
@@ -6560,7 +6559,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>59</v>
       </c>
@@ -6660,7 +6659,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>60</v>
       </c>
@@ -6760,7 +6759,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>52</v>
       </c>
@@ -6858,7 +6857,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
@@ -6958,7 +6957,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>54</v>
       </c>
@@ -7458,7 +7457,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>63</v>
       </c>
@@ -7558,7 +7557,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>91</v>
       </c>
@@ -7658,7 +7657,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>92</v>
       </c>
@@ -7758,7 +7757,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -7858,7 +7857,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>94</v>
       </c>
@@ -7958,7 +7957,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>64</v>
       </c>
@@ -8056,7 +8055,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
         <v>65</v>
       </c>
@@ -8156,7 +8155,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>70</v>
       </c>
@@ -8462,7 +8461,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>66</v>
       </c>
@@ -8564,7 +8563,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="43" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>68</v>
       </c>
@@ -8664,7 +8663,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="44" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>67</v>
       </c>
@@ -8766,7 +8765,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>69</v>
       </c>
@@ -8966,7 +8965,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>86</v>
       </c>
@@ -9064,7 +9063,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>90</v>
       </c>
@@ -9162,7 +9161,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>88</v>
       </c>
@@ -9260,7 +9259,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="50" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>89</v>
       </c>
@@ -9358,7 +9357,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
         <v>87</v>
       </c>
@@ -9456,7 +9455,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>84</v>
       </c>
@@ -9556,7 +9555,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>367</v>
       </c>
@@ -9640,7 +9639,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="54" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>85</v>
       </c>
@@ -9740,7 +9739,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="55" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>121</v>
       </c>
@@ -9842,7 +9841,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="56" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>120</v>
       </c>
@@ -9942,7 +9941,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="57" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>100</v>
       </c>
@@ -10040,7 +10039,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="58" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
         <v>101</v>
       </c>
@@ -10140,7 +10139,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>104</v>
       </c>
@@ -10240,7 +10239,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="60" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>387</v>
       </c>
@@ -10326,7 +10325,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="61" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>390</v>
       </c>
@@ -10412,7 +10411,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="62" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
         <v>394</v>
       </c>
@@ -10498,7 +10497,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="63" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
         <v>106</v>
       </c>
@@ -10598,7 +10597,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="64" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
         <v>400</v>
       </c>
@@ -10682,7 +10681,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="65" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
         <v>105</v>
       </c>
@@ -10782,7 +10781,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="66" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>107</v>
       </c>
@@ -10880,7 +10879,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="67" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
         <v>108</v>
       </c>
@@ -10980,7 +10979,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="68" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
         <v>109</v>
       </c>
@@ -11078,7 +11077,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="69" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
         <v>416</v>
       </c>
@@ -11164,7 +11163,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="70" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
         <v>103</v>
       </c>
@@ -11264,7 +11263,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="71" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
         <v>102</v>
       </c>
@@ -11364,7 +11363,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="72" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
         <v>110</v>
       </c>
@@ -11464,7 +11463,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
         <v>111</v>
       </c>
@@ -11562,7 +11561,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="74" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
         <v>112</v>
       </c>
@@ -11662,7 +11661,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="75" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>113</v>
       </c>
@@ -11760,7 +11759,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="76" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>437</v>
       </c>
@@ -11844,7 +11843,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="77" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>114</v>
       </c>
@@ -11944,7 +11943,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="78" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>115</v>
       </c>
@@ -12042,7 +12041,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="79" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
         <v>116</v>
       </c>
@@ -12140,7 +12139,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="80" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>117</v>
       </c>
@@ -12240,7 +12239,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="81" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>118</v>
       </c>
@@ -12340,7 +12339,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="82" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>454</v>
       </c>
@@ -12424,7 +12423,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="83" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>122</v>
       </c>
@@ -12522,7 +12521,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="84" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>123</v>
       </c>
@@ -12622,7 +12621,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="85" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
         <v>124</v>
       </c>
@@ -12724,7 +12723,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="86" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
         <v>467</v>
       </c>
@@ -12808,7 +12807,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="87" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
         <v>125</v>
       </c>
@@ -12906,7 +12905,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="88" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
         <v>126</v>
       </c>
@@ -13004,7 +13003,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="89" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
         <v>127</v>
       </c>
@@ -13104,7 +13103,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="90" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>73</v>
       </c>
@@ -13204,7 +13203,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="91" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A91" s="17" t="s">
         <v>82</v>
       </c>
@@ -13304,7 +13303,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="92" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>74</v>
       </c>
@@ -13404,7 +13403,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="93" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A93" s="17" t="s">
         <v>75</v>
       </c>
@@ -13690,7 +13689,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="96" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A96" s="17" t="s">
         <v>77</v>
       </c>
@@ -13790,7 +13789,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="97" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A97" s="17" t="s">
         <v>78</v>
       </c>
@@ -14090,7 +14089,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="100" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A100" s="17" t="s">
         <v>81</v>
       </c>
@@ -14192,7 +14191,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="101" spans="1:35" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A101" s="17" t="s">
         <v>83</v>
       </c>
@@ -14295,18 +14294,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI101" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="20">
-      <filters>
-        <filter val="NPT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
edits to Salmon and Clearwater chnk MPGs
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230814.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230814.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F91B86C-959D-4195-9602-B1A82680D5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2E23A0-3FEF-4931-84E4-C9B4A1740444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36705" yWindow="1695" windowWidth="12150" windowHeight="11370" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="581" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -4419,7 +4419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
   <dimension ref="A1:AI104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -14616,11 +14616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175A1EF7-D6F6-40B5-8CC5-720EBF0869DB}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15949,8 +15949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B48E5-B2D0-4B19-967E-72BE4D4B4F25}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>